<commit_message>
Replace files with newer version
Remove some files, change some files.
As a side effect, the file modes are apparently all changed, but the
contents are oftentimes identical to what was before.
</commit_message>
<xml_diff>
--- a/SmartHomeGUI/misc/Studien-Evaluierung1.xlsx
+++ b/SmartHomeGUI/misc/Studien-Evaluierung1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="46">
   <si>
     <t>Walllights OFF</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>&gt;50 sec</t>
+  </si>
+  <si>
+    <t>3D zuerst</t>
+  </si>
+  <si>
+    <t>2D zuerst</t>
   </si>
 </sst>
 </file>
@@ -423,39 +429,11 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -479,31 +457,6 @@
           <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -803,7 +756,7 @@
   <dimension ref="A1:Y72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -931,6 +884,9 @@
       <c r="K9" s="12">
         <v>31</v>
       </c>
+      <c r="M9" t="s">
+        <v>44</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1553,7 +1509,9 @@
         <v>32</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -2178,20 +2136,20 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="19">
-        <f>AVERAGE(B11,D11,F11,H11,J11,J23,H23,F23,D23,B23)</f>
+        <f t="shared" ref="M36:N41" si="35">AVERAGE(B11,D11,F11,H11,J11,J23,H23,F23,D23,B23)</f>
         <v>11.579999999999998</v>
       </c>
       <c r="N36" s="30">
-        <f>AVERAGE(C11,E11,G11,I11,K11,K23,I23,G23,E23,C23)</f>
+        <f t="shared" si="35"/>
         <v>28.190999999999995</v>
       </c>
       <c r="O36" s="16"/>
       <c r="P36" s="19">
-        <f>MEDIAN(B11,D11,F11,H11,J11,B23,D23,F23,H23,J23)</f>
+        <f t="shared" ref="P36:Q41" si="36">MEDIAN(B11,D11,F11,H11,J11,B23,D23,F23,H23,J23)</f>
         <v>10.65</v>
       </c>
       <c r="Q36" s="30">
-        <f>MEDIAN(C11,E11,G11,I11,K11,C23,E23,G23,I23,K23)</f>
+        <f t="shared" si="36"/>
         <v>24.15</v>
       </c>
       <c r="R36" s="1"/>
@@ -2208,20 +2166,20 @@
         <v>0</v>
       </c>
       <c r="M37" s="19">
-        <f>AVERAGE(B12,D12,F12,H12,J12,J24,H24,F24,D24,B24)</f>
+        <f t="shared" si="35"/>
         <v>2.68</v>
       </c>
       <c r="N37" s="30">
-        <f>AVERAGE(C12,E12,G12,I12,K12,K24,I24,G24,E24,C24)</f>
+        <f t="shared" si="35"/>
         <v>5.488999999999999</v>
       </c>
       <c r="O37" s="16"/>
       <c r="P37" s="19">
-        <f>MEDIAN(B12,D12,F12,H12,J12,B24,D24,F24,H24,J24)</f>
+        <f t="shared" si="36"/>
         <v>2.5</v>
       </c>
       <c r="Q37" s="30">
-        <f>MEDIAN(C12,E12,G12,I12,K12,C24,E24,G24,I24,K24)</f>
+        <f t="shared" si="36"/>
         <v>5.6</v>
       </c>
       <c r="R37" s="1"/>
@@ -2238,20 +2196,20 @@
         <v>2</v>
       </c>
       <c r="M38" s="19">
-        <f>AVERAGE(B13,D13,F13,H13,J13,J25,H25,F25,D25,B25)</f>
+        <f t="shared" si="35"/>
         <v>13.3</v>
       </c>
       <c r="N38" s="30">
-        <f>AVERAGE(C13,E13,G13,I13,K13,K25,I25,G25,E25,C25)</f>
+        <f t="shared" si="35"/>
         <v>10.409000000000001</v>
       </c>
       <c r="O38" s="16"/>
       <c r="P38" s="19">
-        <f>MEDIAN(B13,D13,F13,H13,J13,B25,D25,F25,H25,J25)</f>
+        <f t="shared" si="36"/>
         <v>9.85</v>
       </c>
       <c r="Q38" s="30">
-        <f>MEDIAN(C13,E13,G13,I13,K13,C25,E25,G25,I25,K25)</f>
+        <f t="shared" si="36"/>
         <v>9.5500000000000007</v>
       </c>
       <c r="R38" s="1"/>
@@ -2268,20 +2226,20 @@
         <v>3</v>
       </c>
       <c r="M39" s="19">
-        <f>AVERAGE(B14,D14,F14,H14,J14,J26,H26,F26,D26,B26)</f>
+        <f t="shared" si="35"/>
         <v>7.17</v>
       </c>
       <c r="N39" s="30">
-        <f>AVERAGE(C14,E14,G14,I14,K14,K26,I26,G26,E26,C26)</f>
+        <f t="shared" si="35"/>
         <v>6.01</v>
       </c>
       <c r="O39" s="16"/>
       <c r="P39" s="19">
-        <f>MEDIAN(B14,D14,F14,H14,J14,B26,D26,F26,H26,J26)</f>
+        <f t="shared" si="36"/>
         <v>7.1</v>
       </c>
       <c r="Q39" s="30">
-        <f>MEDIAN(C14,E14,G14,I14,K14,C26,E26,G26,I26,K26)</f>
+        <f t="shared" si="36"/>
         <v>5.45</v>
       </c>
       <c r="R39" s="1"/>
@@ -2298,20 +2256,20 @@
         <v>4</v>
       </c>
       <c r="M40" s="19">
-        <f>AVERAGE(B15,D15,F15,H15,J15,J27,H27,F27,D27,B27)</f>
+        <f t="shared" si="35"/>
         <v>7.8059999999999992</v>
       </c>
       <c r="N40" s="30">
-        <f>AVERAGE(C15,E15,G15,I15,K15,K27,I27,G27,E27,C27)</f>
+        <f t="shared" si="35"/>
         <v>12.7</v>
       </c>
       <c r="O40" s="16"/>
       <c r="P40" s="19">
-        <f>MEDIAN(B15,D15,F15,H15,J15,B27,D27,F27,H27,J27)</f>
+        <f t="shared" si="36"/>
         <v>7.38</v>
       </c>
       <c r="Q40" s="30">
-        <f>MEDIAN(C15,E15,G15,I15,K15,C27,E27,G27,I27,K27)</f>
+        <f t="shared" si="36"/>
         <v>8.6499999999999986</v>
       </c>
       <c r="R40" s="1"/>
@@ -2339,20 +2297,20 @@
       <c r="K41" s="39"/>
       <c r="L41" s="36"/>
       <c r="M41" s="19">
-        <f>AVERAGE(B16,D16,F16,H16,J16,J28,H28,F28,D28,B28)</f>
+        <f t="shared" si="35"/>
         <v>4.32</v>
       </c>
       <c r="N41" s="31">
-        <f>AVERAGE(C16,E16,G16,I16,K16,K28,I28,G28,E28,C28)</f>
+        <f t="shared" si="35"/>
         <v>5.9999999999999991</v>
       </c>
       <c r="O41" s="16"/>
       <c r="P41" s="19">
-        <f>MEDIAN(B16,D16,F16,H16,J16,B28,D28,F28,H28,J28)</f>
+        <f t="shared" si="36"/>
         <v>4.05</v>
       </c>
       <c r="Q41" s="31">
-        <f>MEDIAN(C16,E16,G16,I16,K16,C28,E28,G28,I28,K28)</f>
+        <f t="shared" si="36"/>
         <v>5.4499999999999993</v>
       </c>
       <c r="R41" s="1"/>
@@ -2380,20 +2338,20 @@
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
       <c r="M42" s="28">
-        <f t="shared" ref="M42:N42" si="35">AVERAGE(M36:M41)</f>
+        <f t="shared" ref="M42:N42" si="37">AVERAGE(M36:M41)</f>
         <v>7.8093333333333321</v>
       </c>
       <c r="N42" s="28">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>11.466499999999998</v>
       </c>
       <c r="O42" s="17"/>
       <c r="P42" s="28">
-        <f t="shared" ref="P42:Q42" si="36">AVERAGE(P36:P41)</f>
+        <f t="shared" ref="P42:Q42" si="38">AVERAGE(P36:P41)</f>
         <v>6.9216666666666669</v>
       </c>
       <c r="Q42" s="28">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>9.8083333333333318</v>
       </c>
       <c r="R42" s="1"/>
@@ -2412,7 +2370,7 @@
         <v>31</v>
       </c>
       <c r="N43" s="32">
-        <f t="shared" ref="N43" si="37">M42-N42</f>
+        <f t="shared" ref="N43" si="39">M42-N42</f>
         <v>-3.657166666666666</v>
       </c>
       <c r="O43" s="1"/>
@@ -2420,7 +2378,7 @@
         <v>31</v>
       </c>
       <c r="Q43" s="32">
-        <f t="shared" ref="Q43" si="38">P42-Q42</f>
+        <f t="shared" ref="Q43" si="40">P42-Q42</f>
         <v>-2.8866666666666649</v>
       </c>
       <c r="R43" s="1"/>
@@ -2502,7 +2460,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" ref="D46" si="39">COUNTIF($B$11:$K$16,"&gt;20")</f>
+        <f t="shared" ref="D46" si="41">COUNTIF($B$11:$K$16,"&gt;20")</f>
         <v>8</v>
       </c>
       <c r="E46" s="3">
@@ -2606,31 +2564,31 @@
         <v>20</v>
       </c>
       <c r="D48" s="40">
-        <f t="shared" ref="D48:J48" si="40">SUM(D46:D47)</f>
+        <f t="shared" ref="D48:J48" si="42">SUM(D46:D47)</f>
         <v>12</v>
       </c>
       <c r="E48" s="40">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>8</v>
       </c>
       <c r="F48" s="40">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>5</v>
       </c>
       <c r="G48" s="40">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>5</v>
       </c>
       <c r="H48" s="40">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>3</v>
       </c>
       <c r="I48" s="40">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="J48" s="38">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="K48" s="1"/>
@@ -4635,14 +4593,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:K29 B17:K17">
-    <cfRule type="top10" dxfId="7" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17 B29:K29">
-    <cfRule type="top10" dxfId="6" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:K16 B23:K28">
-    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>